<commit_message>
Fixed formatting in excel file
</commit_message>
<xml_diff>
--- a/LASAN.xlsx
+++ b/LASAN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Desktop\lariver_waterlevels\lariver_waterlevels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EEB28A0-8B87-4193-BDAE-6CFFDFA43778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34526EA4-36D8-4544-8C02-3A3E8CA29DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{380A2BCC-CBAB-4C17-9304-59873BD3077B}"/>
+    <workbookView xWindow="0" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{380A2BCC-CBAB-4C17-9304-59873BD3077B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -525,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1948CA7F-223A-41D9-8906-E3EB2B30C256}">
   <dimension ref="A1:C3963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3912" workbookViewId="0">
-      <selection sqref="A1:C3963"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1689,146 +1710,146 @@
         <v>19.001908800000002</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
         <v>45546.097222222219</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="4">
         <v>19.008656000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
         <v>45546.100694444445</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="4">
         <v>18.944606399999998</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="3">
         <v>45546.104166666664</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="4">
         <v>18.570928000000002</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
         <v>45546.107638888891</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="4">
         <v>0</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="4">
         <v>18.917566399999998</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
         <v>45546.111111111109</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="4">
         <v>0</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="4">
         <v>18.906436800000002</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
         <v>45546.114583333336</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="4">
         <v>18.914624</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
         <v>45546.118055555555</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="4">
         <v>-0.01</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="4">
         <v>18.873815999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
         <v>45546.121527777781</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="4">
         <v>18.900572799999999</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
         <v>45546.125</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="4">
         <v>-0.01</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="4">
         <v>18.856092799999999</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
         <v>45546.128472222219</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="4">
         <v>18.8225856</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
         <v>45546.131944444445</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="4">
         <v>18.8052496</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A117">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
         <v>45546.135416666664</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="4">
         <v>18.771547200000001</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A118">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
         <v>45546.138888888891</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="4">
         <v>-0.02</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="4">
         <v>18.7471408</v>
       </c>
     </row>
@@ -44129,11 +44150,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C77 A366:C653 A942:C1229 A1518:C1805 A2095:C2381 A2670:C2957 A3246:C3533 A3822:C3963">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A78:C105 A119:C365 A654:C941 A1230:C1517 A1806:C2094 A2382:C2669 A2958:C3245 A3534:C3821">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A106:A118">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B106:B118">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A78:C105 A654:C941 A1230:C1517 A1806:C2094 A2382:C2669 A2958:C3245 A3534:C3821 A119:C365">
+  <conditionalFormatting sqref="C106:C118">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>